<commit_message>
creating and deleting game/user with categories and questions now works
</commit_message>
<xml_diff>
--- a/doc/Definitions.xlsx
+++ b/doc/Definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aron\Projects\jeopardy\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AE6FBBF-EE7B-4969-B616-01A11A3C2A2D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5B0C5A46-A4D9-4C8E-A079-59E694052EEC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
   <si>
     <t>Klassen</t>
   </si>
@@ -79,9 +79,6 @@
     <t>creator</t>
   </si>
   <si>
-    <t>color</t>
-  </si>
-  <si>
     <t>video?</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>bg-image</t>
   </si>
   <si>
     <t>picture?</t>
@@ -599,7 +593,9 @@
   </sheetPr>
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -607,7 +603,7 @@
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,83 +731,75 @@
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,206 +807,206 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E36" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>